<commit_message>
20231009_latest class work exercises & CA1 progress
</commit_message>
<xml_diff>
--- a/s1_ca1/outputs/output_review.xlsx
+++ b/s1_ca1/outputs/output_review.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shass\my_github\cct_msc_data_analytics\s1_ca1\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657135A6-086D-4043-B427-955EBD165761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F1D6BF-5945-42E5-A9C2-160D3B0E1C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pop_change_df" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="pop_est_df" sheetId="7" r:id="rId3"/>
     <sheet name="pop_est_pivot_df" sheetId="2" r:id="rId4"/>
     <sheet name="gdp_gnp_df" sheetId="10" r:id="rId5"/>
-    <sheet name="gdp_gnp_pivot_df" sheetId="4" r:id="rId6"/>
+    <sheet name="gdp_gnp_pivot_df" sheetId="11" r:id="rId6"/>
+    <sheet name="outer_merged_df" sheetId="14" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1544" uniqueCount="50">
   <si>
     <t>Male</t>
   </si>
@@ -151,6 +152,36 @@
   <si>
     <t>Sex</t>
   </si>
+  <si>
+    <t>GDP</t>
+  </si>
+  <si>
+    <t>GNP</t>
+  </si>
+  <si>
+    <t>GVA</t>
+  </si>
+  <si>
+    <t>Population Change</t>
+  </si>
+  <si>
+    <t>Annual Births</t>
+  </si>
+  <si>
+    <t>Annual Deaths</t>
+  </si>
+  <si>
+    <t>Natural Increase</t>
+  </si>
+  <si>
+    <t>Net Migration</t>
+  </si>
+  <si>
+    <t>Both Sexes</t>
+  </si>
+  <si>
+    <t>Increase</t>
+  </si>
 </sst>
 </file>
 
@@ -216,10 +247,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,6 +566,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{074DEFD1-BE3A-4855-B0A8-245C67D72B67}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C585"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6558,7 +6591,8 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I26"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6574,11 +6608,12 @@
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -6601,13 +6636,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1998</v>
       </c>
@@ -6630,13 +6668,17 @@
         <v>17400</v>
       </c>
       <c r="H2">
+        <f>F2+G2</f>
+        <v>38900</v>
+      </c>
+      <c r="I2">
         <v>3703100</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>38800</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1999</v>
       </c>
@@ -6659,13 +6701,17 @@
         <v>17300</v>
       </c>
       <c r="H3">
+        <f t="shared" ref="H3:H26" si="0">F3+G3</f>
+        <v>38500</v>
+      </c>
+      <c r="I3">
         <v>3741600</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>38500</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2000</v>
       </c>
@@ -6688,13 +6734,17 @@
         <v>26000</v>
       </c>
       <c r="H4">
+        <f t="shared" si="0"/>
+        <v>47800</v>
+      </c>
+      <c r="I4">
         <v>3789500</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>47900</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2001</v>
       </c>
@@ -6717,13 +6767,17 @@
         <v>32800</v>
       </c>
       <c r="H5">
+        <f t="shared" si="0"/>
+        <v>57600</v>
+      </c>
+      <c r="I5">
         <v>3847200</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>57700</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2002</v>
       </c>
@@ -6746,13 +6800,17 @@
         <v>41300</v>
       </c>
       <c r="H6">
+        <f t="shared" si="0"/>
+        <v>70100</v>
+      </c>
+      <c r="I6">
         <v>3917200</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>70000</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2003</v>
       </c>
@@ -6775,13 +6833,17 @@
         <v>30700</v>
       </c>
       <c r="H7">
+        <f t="shared" si="0"/>
+        <v>62600</v>
+      </c>
+      <c r="I7">
         <v>3979900</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>62600</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2004</v>
       </c>
@@ -6804,13 +6866,17 @@
         <v>32000</v>
       </c>
       <c r="H8">
+        <f t="shared" si="0"/>
+        <v>65300</v>
+      </c>
+      <c r="I8">
         <v>4045200</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>65300</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2005</v>
       </c>
@@ -6833,13 +6899,17 @@
         <v>55100</v>
       </c>
       <c r="H9">
+        <f t="shared" si="0"/>
+        <v>88600</v>
+      </c>
+      <c r="I9">
         <v>4133800</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>88600</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2006</v>
       </c>
@@ -6862,13 +6932,17 @@
         <v>71800</v>
       </c>
       <c r="H10">
+        <f t="shared" si="0"/>
+        <v>106000</v>
+      </c>
+      <c r="I10">
         <v>4232900</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>106000</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2007</v>
       </c>
@@ -6891,13 +6965,17 @@
         <v>104800</v>
       </c>
       <c r="H11">
+        <f t="shared" si="0"/>
+        <v>143000</v>
+      </c>
+      <c r="I11">
         <v>4375800</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>142900</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2008</v>
       </c>
@@ -6920,13 +6998,17 @@
         <v>64300</v>
       </c>
       <c r="H12">
+        <f t="shared" si="0"/>
+        <v>109200</v>
+      </c>
+      <c r="I12">
         <v>4485100</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>109200</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2009</v>
       </c>
@@ -6949,13 +7031,17 @@
         <v>1600</v>
       </c>
       <c r="H13">
+        <f t="shared" si="0"/>
+        <v>48300</v>
+      </c>
+      <c r="I13">
         <v>4533400</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>48300</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2010</v>
       </c>
@@ -6978,13 +7064,17 @@
         <v>-27500</v>
       </c>
       <c r="H14">
+        <f t="shared" si="0"/>
+        <v>21300</v>
+      </c>
+      <c r="I14">
         <v>4554800</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>21400</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2011</v>
       </c>
@@ -7007,13 +7097,17 @@
         <v>-27400</v>
       </c>
       <c r="H15">
+        <f t="shared" si="0"/>
+        <v>20100</v>
+      </c>
+      <c r="I15">
         <v>4574900</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>20100</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2012</v>
       </c>
@@ -7036,13 +7130,17 @@
         <v>-25700</v>
       </c>
       <c r="H16">
+        <f t="shared" si="0"/>
+        <v>18800</v>
+      </c>
+      <c r="I16">
         <v>4593700</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>18800</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2013</v>
       </c>
@@ -7065,13 +7163,17 @@
         <v>-18700</v>
       </c>
       <c r="H17">
+        <f t="shared" si="0"/>
+        <v>20900</v>
+      </c>
+      <c r="I17">
         <v>4614700</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>21000</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2014</v>
       </c>
@@ -7094,13 +7196,17 @@
         <v>-8500</v>
       </c>
       <c r="H18">
+        <f t="shared" si="0"/>
+        <v>30700</v>
+      </c>
+      <c r="I18">
         <v>4645400</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>30800</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2015</v>
       </c>
@@ -7123,13 +7229,17 @@
         <v>5900</v>
       </c>
       <c r="H19">
+        <f t="shared" si="0"/>
+        <v>42400</v>
+      </c>
+      <c r="I19">
         <v>4687800</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>42300</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2016</v>
       </c>
@@ -7152,13 +7262,17 @@
         <v>16200</v>
       </c>
       <c r="H20">
+        <f t="shared" si="0"/>
+        <v>51800</v>
+      </c>
+      <c r="I20">
         <v>4739600</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>51800</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2017</v>
       </c>
@@ -7181,13 +7295,17 @@
         <v>39200</v>
       </c>
       <c r="H21">
+        <f t="shared" si="0"/>
+        <v>71300</v>
+      </c>
+      <c r="I21">
         <v>4810900</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>71300</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2018</v>
       </c>
@@ -7210,13 +7328,17 @@
         <v>44400</v>
       </c>
       <c r="H22">
+        <f t="shared" si="0"/>
+        <v>74000</v>
+      </c>
+      <c r="I22">
         <v>4884900</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>74000</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2019</v>
       </c>
@@ -7239,13 +7361,17 @@
         <v>44000</v>
       </c>
       <c r="H23">
+        <f t="shared" si="0"/>
+        <v>73600</v>
+      </c>
+      <c r="I23">
         <v>4958500</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>73600</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2020</v>
       </c>
@@ -7268,13 +7394,17 @@
         <v>44700</v>
       </c>
       <c r="H24">
+        <f t="shared" si="0"/>
+        <v>71400</v>
+      </c>
+      <c r="I24">
         <v>5029900</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>71400</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2021</v>
       </c>
@@ -7297,13 +7427,17 @@
         <v>21800</v>
       </c>
       <c r="H25">
+        <f t="shared" si="0"/>
+        <v>44800</v>
+      </c>
+      <c r="I25">
         <v>5074700</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>44800</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2022</v>
       </c>
@@ -7326,9 +7460,13 @@
         <v>51700</v>
       </c>
       <c r="H26">
+        <f t="shared" si="0"/>
+        <v>77800</v>
+      </c>
+      <c r="I26">
         <v>5184000</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>77800</v>
       </c>
     </row>
@@ -7339,6 +7477,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{887B7D52-D0B0-476C-AB45-1ECC015DD5DE}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C223"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9813,6 +9952,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10195,6 +10335,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1A07EA3-E0C6-432E-8B7C-603AD29AB4B2}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C697"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17882,8 +18023,393 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8CC8A2-B95A-4133-9439-5D21010715A4}">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1998</v>
+      </c>
+      <c r="B2">
+        <v>125594000000</v>
+      </c>
+      <c r="C2">
+        <v>117567000000</v>
+      </c>
+      <c r="D2">
+        <v>112817000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1999</v>
+      </c>
+      <c r="B3">
+        <v>138819000000</v>
+      </c>
+      <c r="C3">
+        <v>127088000000</v>
+      </c>
+      <c r="D3">
+        <v>123893000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2000</v>
+      </c>
+      <c r="B4">
+        <v>151873000000</v>
+      </c>
+      <c r="C4">
+        <v>138791000000</v>
+      </c>
+      <c r="D4">
+        <v>135161000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2001</v>
+      </c>
+      <c r="B5">
+        <v>159932000000</v>
+      </c>
+      <c r="C5">
+        <v>141356000000</v>
+      </c>
+      <c r="D5">
+        <v>143313000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2002</v>
+      </c>
+      <c r="B6">
+        <v>169366000000</v>
+      </c>
+      <c r="C6">
+        <v>144707000000</v>
+      </c>
+      <c r="D6">
+        <v>152258000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2003</v>
+      </c>
+      <c r="B7">
+        <v>174471000000</v>
+      </c>
+      <c r="C7">
+        <v>151555000000</v>
+      </c>
+      <c r="D7">
+        <v>156260000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2004</v>
+      </c>
+      <c r="B8">
+        <v>186315000000</v>
+      </c>
+      <c r="C8">
+        <v>162276000000</v>
+      </c>
+      <c r="D8">
+        <v>166155000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2005</v>
+      </c>
+      <c r="B9">
+        <v>197008000000</v>
+      </c>
+      <c r="C9">
+        <v>171101000000</v>
+      </c>
+      <c r="D9">
+        <v>174006000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2006</v>
+      </c>
+      <c r="B10">
+        <v>206834000000</v>
+      </c>
+      <c r="C10">
+        <v>180814000000</v>
+      </c>
+      <c r="D10">
+        <v>181212000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2007</v>
+      </c>
+      <c r="B11">
+        <v>217818000000</v>
+      </c>
+      <c r="C11">
+        <v>187527000000</v>
+      </c>
+      <c r="D11">
+        <v>192763000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2008</v>
+      </c>
+      <c r="B12">
+        <v>208051000000</v>
+      </c>
+      <c r="C12">
+        <v>180139000000</v>
+      </c>
+      <c r="D12">
+        <v>187712000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2009</v>
+      </c>
+      <c r="B13">
+        <v>197450000000</v>
+      </c>
+      <c r="C13">
+        <v>165003000000</v>
+      </c>
+      <c r="D13">
+        <v>180811000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2010</v>
+      </c>
+      <c r="B14">
+        <v>200772000000</v>
+      </c>
+      <c r="C14">
+        <v>171011000000</v>
+      </c>
+      <c r="D14">
+        <v>184048000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2011</v>
+      </c>
+      <c r="B15">
+        <v>203343000000</v>
+      </c>
+      <c r="C15">
+        <v>166763000000</v>
+      </c>
+      <c r="D15">
+        <v>187495000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2012</v>
+      </c>
+      <c r="B16">
+        <v>203080000000</v>
+      </c>
+      <c r="C16">
+        <v>166053000000</v>
+      </c>
+      <c r="D16">
+        <v>187102000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2013</v>
+      </c>
+      <c r="B17">
+        <v>205466000000</v>
+      </c>
+      <c r="C17">
+        <v>175230000000</v>
+      </c>
+      <c r="D17">
+        <v>188780000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2014</v>
+      </c>
+      <c r="B18">
+        <v>223606000000</v>
+      </c>
+      <c r="C18">
+        <v>191298000000</v>
+      </c>
+      <c r="D18">
+        <v>205224000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2015</v>
+      </c>
+      <c r="B19">
+        <v>278334000000</v>
+      </c>
+      <c r="C19">
+        <v>215863000000</v>
+      </c>
+      <c r="D19">
+        <v>258944000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2016</v>
+      </c>
+      <c r="B20">
+        <v>283248000000</v>
+      </c>
+      <c r="C20">
+        <v>231361000000</v>
+      </c>
+      <c r="D20">
+        <v>262607000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2017</v>
+      </c>
+      <c r="B21">
+        <v>309621000000</v>
+      </c>
+      <c r="C21">
+        <v>246086000000</v>
+      </c>
+      <c r="D21">
+        <v>288222000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2018</v>
+      </c>
+      <c r="B22">
+        <v>335849000000</v>
+      </c>
+      <c r="C22">
+        <v>260724000000</v>
+      </c>
+      <c r="D22">
+        <v>313888000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2019</v>
+      </c>
+      <c r="B23">
+        <v>353641000000</v>
+      </c>
+      <c r="C23">
+        <v>273940000000</v>
+      </c>
+      <c r="D23">
+        <v>330084000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2020</v>
+      </c>
+      <c r="B24">
+        <v>377042000000</v>
+      </c>
+      <c r="C24">
+        <v>283779000000</v>
+      </c>
+      <c r="D24">
+        <v>356769000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2021</v>
+      </c>
+      <c r="B25">
+        <v>434069000000</v>
+      </c>
+      <c r="C25">
+        <v>323313000000</v>
+      </c>
+      <c r="D25">
+        <v>409387000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2022</v>
+      </c>
+      <c r="B26">
+        <v>475016000000</v>
+      </c>
+      <c r="C26">
+        <v>335904000000</v>
+      </c>
+      <c r="D26">
+        <v>450216000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B73FEC4-C860-4D66-9DE4-6E40B33C385A}">
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -17893,2032 +18419,1239 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="46.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="55.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="50.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="71.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="72.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="56.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="53" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1998</v>
       </c>
       <c r="B2">
+        <v>3703100</v>
+      </c>
+      <c r="C2">
+        <v>38900</v>
+      </c>
+      <c r="D2">
+        <v>52700</v>
+      </c>
+      <c r="E2">
+        <v>31200</v>
+      </c>
+      <c r="F2">
+        <v>21500</v>
+      </c>
+      <c r="G2">
+        <v>46000</v>
+      </c>
+      <c r="H2">
+        <v>28600</v>
+      </c>
+      <c r="I2">
+        <v>17400</v>
+      </c>
+      <c r="J2">
+        <v>1838900</v>
+      </c>
+      <c r="K2">
+        <v>1864200</v>
+      </c>
+      <c r="L2">
+        <v>3703100</v>
+      </c>
+      <c r="M2">
         <v>125594000000</v>
       </c>
-      <c r="C2">
-        <v>128240000000</v>
-      </c>
-      <c r="D2">
-        <v>80431000000</v>
-      </c>
-      <c r="E2">
-        <v>80568000000</v>
-      </c>
-      <c r="F2">
+      <c r="N2">
         <v>117567000000</v>
       </c>
-      <c r="G2">
-        <v>117146000000</v>
-      </c>
-      <c r="H2">
-        <v>70880000000</v>
-      </c>
-      <c r="I2">
-        <v>71044000000</v>
-      </c>
-      <c r="J2">
+      <c r="O2">
         <v>112817000000</v>
       </c>
-      <c r="K2">
-        <v>115760000000</v>
-      </c>
-      <c r="L2">
-        <v>72024000000</v>
-      </c>
-      <c r="M2">
-        <v>72118000000</v>
-      </c>
-      <c r="N2">
-        <v>-11148000000</v>
-      </c>
-      <c r="O2">
-        <v>-11092000000</v>
-      </c>
-      <c r="P2">
-        <v>-9550000000</v>
-      </c>
-      <c r="Q2">
-        <v>-9523000000</v>
-      </c>
-      <c r="R2">
-        <v>-2505000000</v>
-      </c>
-      <c r="S2">
-        <v>-2504000000</v>
-      </c>
-      <c r="T2">
-        <v>-1670000000</v>
-      </c>
-      <c r="U2">
-        <v>-1649000000</v>
-      </c>
-      <c r="V2">
-        <v>14951000000</v>
-      </c>
-      <c r="W2">
-        <v>14984000000</v>
-      </c>
-      <c r="X2">
-        <v>10076000000</v>
-      </c>
-      <c r="Y2">
-        <v>10098000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1999</v>
       </c>
       <c r="B3">
+        <v>3741800</v>
+      </c>
+      <c r="C3">
+        <v>38700</v>
+      </c>
+      <c r="D3">
+        <v>53700</v>
+      </c>
+      <c r="E3">
+        <v>32400</v>
+      </c>
+      <c r="F3">
+        <v>21300</v>
+      </c>
+      <c r="G3">
+        <v>48900</v>
+      </c>
+      <c r="H3">
+        <v>31500</v>
+      </c>
+      <c r="I3">
+        <v>17400</v>
+      </c>
+      <c r="J3">
+        <v>1858600</v>
+      </c>
+      <c r="K3">
+        <v>1883000</v>
+      </c>
+      <c r="L3">
+        <v>3741600</v>
+      </c>
+      <c r="M3">
         <v>138819000000</v>
       </c>
-      <c r="C3">
-        <v>141165000000</v>
-      </c>
-      <c r="D3">
-        <v>92791000000</v>
-      </c>
-      <c r="E3">
-        <v>92740000000</v>
-      </c>
-      <c r="F3">
+      <c r="N3">
         <v>127088000000</v>
       </c>
-      <c r="G3">
-        <v>126872000000</v>
-      </c>
-      <c r="H3">
-        <v>79512000000</v>
-      </c>
-      <c r="I3">
-        <v>79471000000</v>
-      </c>
-      <c r="J3">
+      <c r="O3">
         <v>123893000000</v>
       </c>
-      <c r="K3">
-        <v>126608000000</v>
-      </c>
-      <c r="L3">
-        <v>82822000000</v>
-      </c>
-      <c r="M3">
-        <v>82726000000</v>
-      </c>
-      <c r="N3">
-        <v>-14334000000</v>
-      </c>
-      <c r="O3">
-        <v>-14292000000</v>
-      </c>
-      <c r="P3">
-        <v>-13278000000</v>
-      </c>
-      <c r="Q3">
-        <v>-13268000000</v>
-      </c>
-      <c r="R3">
-        <v>-2317000000</v>
-      </c>
-      <c r="S3">
-        <v>-2339000000</v>
-      </c>
-      <c r="T3">
-        <v>-1568000000</v>
-      </c>
-      <c r="U3">
-        <v>-1567000000</v>
-      </c>
-      <c r="V3">
-        <v>16833000000</v>
-      </c>
-      <c r="W3">
-        <v>16896000000</v>
-      </c>
-      <c r="X3">
-        <v>11536000000</v>
-      </c>
-      <c r="Y3">
-        <v>11582000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2000</v>
       </c>
       <c r="B4">
+        <v>3789700</v>
+      </c>
+      <c r="C4">
+        <v>47900</v>
+      </c>
+      <c r="D4">
+        <v>54000</v>
+      </c>
+      <c r="E4">
+        <v>32100</v>
+      </c>
+      <c r="F4">
+        <v>21900</v>
+      </c>
+      <c r="G4">
+        <v>52600</v>
+      </c>
+      <c r="H4">
+        <v>26600</v>
+      </c>
+      <c r="I4">
+        <v>26000</v>
+      </c>
+      <c r="J4">
+        <v>1882900</v>
+      </c>
+      <c r="K4">
+        <v>1906600</v>
+      </c>
+      <c r="L4">
+        <v>3789500</v>
+      </c>
+      <c r="M4">
         <v>151873000000</v>
       </c>
-      <c r="C4">
-        <v>153085000000</v>
-      </c>
-      <c r="D4">
-        <v>108496000000</v>
-      </c>
-      <c r="E4">
-        <v>108137000000</v>
-      </c>
-      <c r="F4">
+      <c r="N4">
         <v>138791000000</v>
       </c>
-      <c r="G4">
-        <v>137248000000</v>
-      </c>
-      <c r="H4">
-        <v>93169000000</v>
-      </c>
-      <c r="I4">
-        <v>92795000000</v>
-      </c>
-      <c r="J4">
+      <c r="O4">
         <v>135161000000</v>
       </c>
-      <c r="K4">
-        <v>136855000000</v>
-      </c>
-      <c r="L4">
-        <v>96723000000</v>
-      </c>
-      <c r="M4">
-        <v>96361000000</v>
-      </c>
-      <c r="N4">
-        <v>-15850000000</v>
-      </c>
-      <c r="O4">
-        <v>-15838000000</v>
-      </c>
-      <c r="P4">
-        <v>-15327000000</v>
-      </c>
-      <c r="Q4">
-        <v>-15339000000</v>
-      </c>
-      <c r="R4">
-        <v>-2303000000</v>
-      </c>
-      <c r="S4">
-        <v>-2327000000</v>
-      </c>
-      <c r="T4">
-        <v>-1643000000</v>
-      </c>
-      <c r="U4">
-        <v>-1646000000</v>
-      </c>
-      <c r="V4">
-        <v>18555000000</v>
-      </c>
-      <c r="W4">
-        <v>18558000000</v>
-      </c>
-      <c r="X4">
-        <v>13416000000</v>
-      </c>
-      <c r="Y4">
-        <v>13422000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2001</v>
       </c>
       <c r="B5">
+        <v>3847400</v>
+      </c>
+      <c r="C5">
+        <v>57700</v>
+      </c>
+      <c r="D5">
+        <v>55100</v>
+      </c>
+      <c r="E5">
+        <v>30200</v>
+      </c>
+      <c r="F5">
+        <v>24900</v>
+      </c>
+      <c r="G5">
+        <v>59000</v>
+      </c>
+      <c r="H5">
+        <v>26200</v>
+      </c>
+      <c r="I5">
+        <v>32800</v>
+      </c>
+      <c r="J5">
+        <v>1913100</v>
+      </c>
+      <c r="K5">
+        <v>1934100</v>
+      </c>
+      <c r="L5">
+        <v>3847200</v>
+      </c>
+      <c r="M5">
         <v>159932000000</v>
       </c>
-      <c r="C5">
-        <v>161749000000</v>
-      </c>
-      <c r="D5">
-        <v>122089000000</v>
-      </c>
-      <c r="E5">
-        <v>121893000000</v>
-      </c>
-      <c r="F5">
+      <c r="N5">
         <v>141356000000</v>
       </c>
-      <c r="G5">
-        <v>141713000000</v>
-      </c>
-      <c r="H5">
-        <v>102947000000</v>
-      </c>
-      <c r="I5">
-        <v>102724000000</v>
-      </c>
-      <c r="J5">
+      <c r="O5">
         <v>143313000000</v>
       </c>
-      <c r="K5">
-        <v>145617000000</v>
-      </c>
-      <c r="L5">
-        <v>109836000000</v>
-      </c>
-      <c r="M5">
-        <v>109638000000</v>
-      </c>
-      <c r="N5">
-        <v>-20022000000</v>
-      </c>
-      <c r="O5">
-        <v>-20035000000</v>
-      </c>
-      <c r="P5">
-        <v>-19142000000</v>
-      </c>
-      <c r="Q5">
-        <v>-19170000000</v>
-      </c>
-      <c r="R5">
-        <v>-1905000000</v>
-      </c>
-      <c r="S5">
-        <v>-1903000000</v>
-      </c>
-      <c r="T5">
-        <v>-1428000000</v>
-      </c>
-      <c r="U5">
-        <v>-1418000000</v>
-      </c>
-      <c r="V5">
-        <v>18052000000</v>
-      </c>
-      <c r="W5">
-        <v>18035000000</v>
-      </c>
-      <c r="X5">
-        <v>13682000000</v>
-      </c>
-      <c r="Y5">
-        <v>13675000000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2002</v>
       </c>
       <c r="B6">
+        <v>3917500</v>
+      </c>
+      <c r="C6">
+        <v>70100</v>
+      </c>
+      <c r="D6">
+        <v>58100</v>
+      </c>
+      <c r="E6">
+        <v>29300</v>
+      </c>
+      <c r="F6">
+        <v>28800</v>
+      </c>
+      <c r="G6">
+        <v>66900</v>
+      </c>
+      <c r="H6">
+        <v>25600</v>
+      </c>
+      <c r="I6">
+        <v>41300</v>
+      </c>
+      <c r="J6">
+        <v>1946200</v>
+      </c>
+      <c r="K6">
+        <v>1971000</v>
+      </c>
+      <c r="L6">
+        <v>3917200</v>
+      </c>
+      <c r="M6">
         <v>169366000000</v>
       </c>
-      <c r="C6">
-        <v>170946000000</v>
-      </c>
-      <c r="D6">
-        <v>135998000000</v>
-      </c>
-      <c r="E6">
-        <v>135858000000</v>
-      </c>
-      <c r="F6">
+      <c r="N6">
         <v>144707000000</v>
       </c>
-      <c r="G6">
-        <v>145889000000</v>
-      </c>
-      <c r="H6">
-        <v>112266000000</v>
-      </c>
-      <c r="I6">
-        <v>112074000000</v>
-      </c>
-      <c r="J6">
+      <c r="O6">
         <v>152258000000</v>
       </c>
-      <c r="K6">
-        <v>154330000000</v>
-      </c>
-      <c r="L6">
-        <v>122822000000</v>
-      </c>
-      <c r="M6">
-        <v>122655000000</v>
-      </c>
-      <c r="N6">
-        <v>-25002000000</v>
-      </c>
-      <c r="O6">
-        <v>-25056000000</v>
-      </c>
-      <c r="P6">
-        <v>-23732000000</v>
-      </c>
-      <c r="Q6">
-        <v>-23785000000</v>
-      </c>
-      <c r="R6">
-        <v>-2400000000</v>
-      </c>
-      <c r="S6">
-        <v>-2382000000</v>
-      </c>
-      <c r="T6">
-        <v>-1894000000</v>
-      </c>
-      <c r="U6">
-        <v>-1864000000</v>
-      </c>
-      <c r="V6">
-        <v>19003000000</v>
-      </c>
-      <c r="W6">
-        <v>18998000000</v>
-      </c>
-      <c r="X6">
-        <v>15070000000</v>
-      </c>
-      <c r="Y6">
-        <v>15066000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2003</v>
       </c>
       <c r="B7">
+        <v>3980100</v>
+      </c>
+      <c r="C7">
+        <v>62600</v>
+      </c>
+      <c r="D7">
+        <v>60800</v>
+      </c>
+      <c r="E7">
+        <v>28900</v>
+      </c>
+      <c r="F7">
+        <v>31900</v>
+      </c>
+      <c r="G7">
+        <v>60000</v>
+      </c>
+      <c r="H7">
+        <v>29300</v>
+      </c>
+      <c r="I7">
+        <v>30700</v>
+      </c>
+      <c r="J7">
+        <v>1976900</v>
+      </c>
+      <c r="K7">
+        <v>2002900</v>
+      </c>
+      <c r="L7">
+        <v>3979800</v>
+      </c>
+      <c r="M7">
         <v>174471000000</v>
       </c>
-      <c r="C7">
-        <v>178082000000</v>
-      </c>
-      <c r="D7">
-        <v>145577000000</v>
-      </c>
-      <c r="E7">
-        <v>145530000000</v>
-      </c>
-      <c r="F7">
+      <c r="N7">
         <v>151555000000</v>
       </c>
-      <c r="G7">
-        <v>154276000000</v>
-      </c>
-      <c r="H7">
-        <v>123807000000</v>
-      </c>
-      <c r="I7">
-        <v>123693000000</v>
-      </c>
-      <c r="J7">
+      <c r="O7">
         <v>156260000000</v>
       </c>
-      <c r="K7">
-        <v>160391000000</v>
-      </c>
-      <c r="L7">
-        <v>131046000000</v>
-      </c>
-      <c r="M7">
-        <v>130997000000</v>
-      </c>
-      <c r="N7">
-        <v>-23724000000</v>
-      </c>
-      <c r="O7">
-        <v>-23806000000</v>
-      </c>
-      <c r="P7">
-        <v>-21770000000</v>
-      </c>
-      <c r="Q7">
-        <v>-21837000000</v>
-      </c>
-      <c r="R7">
-        <v>-2316000000</v>
-      </c>
-      <c r="S7">
-        <v>-2317000000</v>
-      </c>
-      <c r="T7">
-        <v>-1891000000</v>
-      </c>
-      <c r="U7">
-        <v>-1881000000</v>
-      </c>
-      <c r="V7">
-        <v>20017000000</v>
-      </c>
-      <c r="W7">
-        <v>20008000000</v>
-      </c>
-      <c r="X7">
-        <v>16422000000</v>
-      </c>
-      <c r="Y7">
-        <v>16414000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2004</v>
       </c>
       <c r="B8">
+        <v>4045500</v>
+      </c>
+      <c r="C8">
+        <v>65400</v>
+      </c>
+      <c r="D8">
+        <v>62000</v>
+      </c>
+      <c r="E8">
+        <v>28600</v>
+      </c>
+      <c r="F8">
+        <v>33400</v>
+      </c>
+      <c r="G8">
+        <v>58500</v>
+      </c>
+      <c r="H8">
+        <v>26500</v>
+      </c>
+      <c r="I8">
+        <v>32000</v>
+      </c>
+      <c r="J8">
+        <v>2011900</v>
+      </c>
+      <c r="K8">
+        <v>2033300</v>
+      </c>
+      <c r="L8">
+        <v>4045200</v>
+      </c>
+      <c r="M8">
         <v>186315000000</v>
       </c>
-      <c r="C8">
-        <v>189538000000</v>
-      </c>
-      <c r="D8">
-        <v>156259000000</v>
-      </c>
-      <c r="E8">
-        <v>156124000000</v>
-      </c>
-      <c r="F8">
+      <c r="N8">
         <v>162276000000</v>
       </c>
-      <c r="G8">
-        <v>164513000000</v>
-      </c>
-      <c r="H8">
-        <v>133268000000</v>
-      </c>
-      <c r="I8">
-        <v>133078000000</v>
-      </c>
-      <c r="J8">
+      <c r="O8">
         <v>166155000000</v>
       </c>
-      <c r="K8">
-        <v>169900000000</v>
-      </c>
-      <c r="L8">
-        <v>139793000000</v>
-      </c>
-      <c r="M8">
-        <v>139634000000</v>
-      </c>
-      <c r="N8">
-        <v>-24949000000</v>
-      </c>
-      <c r="O8">
-        <v>-25025000000</v>
-      </c>
-      <c r="P8">
-        <v>-22991000000</v>
-      </c>
-      <c r="Q8">
-        <v>-23046000000</v>
-      </c>
-      <c r="R8">
-        <v>-2285000000</v>
-      </c>
-      <c r="S8">
-        <v>-2325000000</v>
-      </c>
-      <c r="T8">
-        <v>-1907000000</v>
-      </c>
-      <c r="U8">
-        <v>-1930000000</v>
-      </c>
-      <c r="V8">
-        <v>21916000000</v>
-      </c>
-      <c r="W8">
-        <v>21962000000</v>
-      </c>
-      <c r="X8">
-        <v>18376000000</v>
-      </c>
-      <c r="Y8">
-        <v>18419000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2005</v>
       </c>
       <c r="B9">
+        <v>4134200</v>
+      </c>
+      <c r="C9">
+        <v>88700</v>
+      </c>
+      <c r="D9">
+        <v>61400</v>
+      </c>
+      <c r="E9">
+        <v>27900</v>
+      </c>
+      <c r="F9">
+        <v>33500</v>
+      </c>
+      <c r="G9">
+        <v>84600</v>
+      </c>
+      <c r="H9">
+        <v>29400</v>
+      </c>
+      <c r="I9">
+        <v>55200</v>
+      </c>
+      <c r="J9">
+        <v>2061800</v>
+      </c>
+      <c r="K9">
+        <v>2072000</v>
+      </c>
+      <c r="L9">
+        <v>4133800</v>
+      </c>
+      <c r="M9">
         <v>197008000000</v>
       </c>
-      <c r="C9">
-        <v>200999000000</v>
-      </c>
-      <c r="D9">
-        <v>170306000000</v>
-      </c>
-      <c r="E9">
-        <v>170364000000</v>
-      </c>
-      <c r="F9">
+      <c r="N9">
         <v>171101000000</v>
       </c>
-      <c r="G9">
-        <v>174100000000</v>
-      </c>
-      <c r="H9">
-        <v>145488000000</v>
-      </c>
-      <c r="I9">
-        <v>145492000000</v>
-      </c>
-      <c r="J9">
+      <c r="O9">
         <v>174006000000</v>
       </c>
-      <c r="K9">
-        <v>178511000000</v>
-      </c>
-      <c r="L9">
-        <v>151023000000</v>
-      </c>
-      <c r="M9">
-        <v>151031000000</v>
-      </c>
-      <c r="N9">
-        <v>-26815000000</v>
-      </c>
-      <c r="O9">
-        <v>-26899000000</v>
-      </c>
-      <c r="P9">
-        <v>-24820000000</v>
-      </c>
-      <c r="Q9">
-        <v>-24872000000</v>
-      </c>
-      <c r="R9">
-        <v>-1597000000</v>
-      </c>
-      <c r="S9">
-        <v>-1586000000</v>
-      </c>
-      <c r="T9">
-        <v>-1365000000</v>
-      </c>
-      <c r="U9">
-        <v>-1350000000</v>
-      </c>
-      <c r="V9">
-        <v>24045000000</v>
-      </c>
-      <c r="W9">
-        <v>24074000000</v>
-      </c>
-      <c r="X9">
-        <v>20648000000</v>
-      </c>
-      <c r="Y9">
-        <v>20685000000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2006</v>
       </c>
       <c r="B10">
+        <v>4240200</v>
+      </c>
+      <c r="C10">
+        <v>106000</v>
+      </c>
+      <c r="D10">
+        <v>61200</v>
+      </c>
+      <c r="E10">
+        <v>27000</v>
+      </c>
+      <c r="F10">
+        <v>34200</v>
+      </c>
+      <c r="G10">
+        <v>107800</v>
+      </c>
+      <c r="H10">
+        <v>36000</v>
+      </c>
+      <c r="I10">
+        <v>71800</v>
+      </c>
+      <c r="J10">
+        <v>2117300</v>
+      </c>
+      <c r="K10">
+        <v>2115600</v>
+      </c>
+      <c r="L10">
+        <v>4232900</v>
+      </c>
+      <c r="M10">
         <v>206834000000</v>
       </c>
-      <c r="C10">
-        <v>211432000000</v>
-      </c>
-      <c r="D10">
-        <v>184916000000</v>
-      </c>
-      <c r="E10">
-        <v>184602000000</v>
-      </c>
-      <c r="F10">
+      <c r="N10">
         <v>180814000000</v>
       </c>
-      <c r="G10">
-        <v>184274000000</v>
-      </c>
-      <c r="H10">
-        <v>160640000000</v>
-      </c>
-      <c r="I10">
-        <v>160265000000</v>
-      </c>
-      <c r="J10">
+      <c r="O10">
         <v>181212000000</v>
       </c>
-      <c r="K10">
-        <v>186407000000</v>
-      </c>
-      <c r="L10">
-        <v>162555000000</v>
-      </c>
-      <c r="M10">
-        <v>162241000000</v>
-      </c>
-      <c r="N10">
-        <v>-27071000000</v>
-      </c>
-      <c r="O10">
-        <v>-27158000000</v>
-      </c>
-      <c r="P10">
-        <v>-24276000000</v>
-      </c>
-      <c r="Q10">
-        <v>-24337000000</v>
-      </c>
-      <c r="R10">
-        <v>-1203000000</v>
-      </c>
-      <c r="S10">
-        <v>-1208000000</v>
-      </c>
-      <c r="T10">
-        <v>-1066000000</v>
-      </c>
-      <c r="U10">
-        <v>-1073000000</v>
-      </c>
-      <c r="V10">
-        <v>26257000000</v>
-      </c>
-      <c r="W10">
-        <v>26234000000</v>
-      </c>
-      <c r="X10">
-        <v>23429000000</v>
-      </c>
-      <c r="Y10">
-        <v>23433000000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2007</v>
       </c>
       <c r="B11">
+        <v>4383200</v>
+      </c>
+      <c r="C11">
+        <v>143000</v>
+      </c>
+      <c r="D11">
+        <v>66600</v>
+      </c>
+      <c r="E11">
+        <v>28400</v>
+      </c>
+      <c r="F11">
+        <v>38200</v>
+      </c>
+      <c r="G11">
+        <v>151100</v>
+      </c>
+      <c r="H11">
+        <v>46300</v>
+      </c>
+      <c r="I11">
+        <v>104800</v>
+      </c>
+      <c r="J11">
+        <v>2191300</v>
+      </c>
+      <c r="K11">
+        <v>2184600</v>
+      </c>
+      <c r="L11">
+        <v>4375900</v>
+      </c>
+      <c r="M11">
         <v>217818000000</v>
       </c>
-      <c r="C11">
-        <v>222452000000</v>
-      </c>
-      <c r="D11">
-        <v>197070000000</v>
-      </c>
-      <c r="E11">
-        <v>196797000000</v>
-      </c>
-      <c r="F11">
+      <c r="N11">
         <v>187527000000</v>
       </c>
-      <c r="G11">
-        <v>190962000000</v>
-      </c>
-      <c r="H11">
-        <v>168920000000</v>
-      </c>
-      <c r="I11">
-        <v>168555000000</v>
-      </c>
-      <c r="J11">
+      <c r="O11">
         <v>192763000000</v>
       </c>
-      <c r="K11">
-        <v>198007000000</v>
-      </c>
-      <c r="L11">
-        <v>174203000000</v>
-      </c>
-      <c r="M11">
-        <v>173927000000</v>
-      </c>
-      <c r="N11">
-        <v>-31370000000</v>
-      </c>
-      <c r="O11">
-        <v>-31489000000</v>
-      </c>
-      <c r="P11">
-        <v>-28149000000</v>
-      </c>
-      <c r="Q11">
-        <v>-28242000000</v>
-      </c>
-      <c r="R11">
-        <v>-1276000000</v>
-      </c>
-      <c r="S11">
-        <v>-1281000000</v>
-      </c>
-      <c r="T11">
-        <v>-1189000000</v>
-      </c>
-      <c r="U11">
-        <v>-1193000000</v>
-      </c>
-      <c r="V11">
-        <v>25724000000</v>
-      </c>
-      <c r="W11">
-        <v>25726000000</v>
-      </c>
-      <c r="X11">
-        <v>24055000000</v>
-      </c>
-      <c r="Y11">
-        <v>24063000000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2008</v>
       </c>
       <c r="B12">
+        <v>4492500</v>
+      </c>
+      <c r="C12">
+        <v>109300</v>
+      </c>
+      <c r="D12">
+        <v>73000</v>
+      </c>
+      <c r="E12">
+        <v>28000</v>
+      </c>
+      <c r="F12">
+        <v>45000</v>
+      </c>
+      <c r="G12">
+        <v>113500</v>
+      </c>
+      <c r="H12">
+        <v>49200</v>
+      </c>
+      <c r="I12">
+        <v>64300</v>
+      </c>
+      <c r="J12">
+        <v>2238600</v>
+      </c>
+      <c r="K12">
+        <v>2246500</v>
+      </c>
+      <c r="L12">
+        <v>4485100</v>
+      </c>
+      <c r="M12">
         <v>208051000000</v>
       </c>
-      <c r="C12">
-        <v>212843000000</v>
-      </c>
-      <c r="D12">
-        <v>187283000000</v>
-      </c>
-      <c r="E12">
-        <v>187182000000</v>
-      </c>
-      <c r="F12">
+      <c r="N12">
         <v>180139000000</v>
       </c>
-      <c r="G12">
-        <v>183825000000</v>
-      </c>
-      <c r="H12">
-        <v>160567000000</v>
-      </c>
-      <c r="I12">
-        <v>160393000000</v>
-      </c>
-      <c r="J12">
+      <c r="O12">
         <v>187712000000</v>
       </c>
-      <c r="K12">
-        <v>193048000000</v>
-      </c>
-      <c r="L12">
-        <v>167950000000</v>
-      </c>
-      <c r="M12">
-        <v>167945000000</v>
-      </c>
-      <c r="N12">
-        <v>-28940000000</v>
-      </c>
-      <c r="O12">
-        <v>-29018000000</v>
-      </c>
-      <c r="P12">
-        <v>-26717000000</v>
-      </c>
-      <c r="Q12">
-        <v>-26788000000</v>
-      </c>
-      <c r="R12">
-        <v>-1316000000</v>
-      </c>
-      <c r="S12">
-        <v>-1327000000</v>
-      </c>
-      <c r="T12">
-        <v>-1277000000</v>
-      </c>
-      <c r="U12">
-        <v>-1286000000</v>
-      </c>
-      <c r="V12">
-        <v>21196000000</v>
-      </c>
-      <c r="W12">
-        <v>21121000000</v>
-      </c>
-      <c r="X12">
-        <v>20610000000</v>
-      </c>
-      <c r="Y12">
-        <v>20521000000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2009</v>
       </c>
       <c r="B13">
+        <v>4540900</v>
+      </c>
+      <c r="C13">
+        <v>48400</v>
+      </c>
+      <c r="D13">
+        <v>75300</v>
+      </c>
+      <c r="E13">
+        <v>28600</v>
+      </c>
+      <c r="F13">
+        <v>46700</v>
+      </c>
+      <c r="G13">
+        <v>73700</v>
+      </c>
+      <c r="H13">
+        <v>72000</v>
+      </c>
+      <c r="I13">
+        <v>1700</v>
+      </c>
+      <c r="J13">
+        <v>2257300</v>
+      </c>
+      <c r="K13">
+        <v>2276100</v>
+      </c>
+      <c r="L13">
+        <v>4533400</v>
+      </c>
+      <c r="M13">
         <v>197450000000</v>
       </c>
-      <c r="C13">
-        <v>201304000000</v>
-      </c>
-      <c r="D13">
-        <v>169520000000</v>
-      </c>
-      <c r="E13">
-        <v>169660000000</v>
-      </c>
-      <c r="F13">
+      <c r="N13">
         <v>165003000000</v>
       </c>
-      <c r="G13">
-        <v>168022000000</v>
-      </c>
-      <c r="H13">
-        <v>140107000000</v>
-      </c>
-      <c r="I13">
-        <v>140186000000</v>
-      </c>
-      <c r="J13">
+      <c r="O13">
         <v>180811000000</v>
       </c>
-      <c r="K13">
-        <v>184891000000</v>
-      </c>
-      <c r="L13">
-        <v>154270000000</v>
-      </c>
-      <c r="M13">
-        <v>154426000000</v>
-      </c>
-      <c r="N13">
-        <v>-33216000000</v>
-      </c>
-      <c r="O13">
-        <v>-33283000000</v>
-      </c>
-      <c r="P13">
-        <v>-29414000000</v>
-      </c>
-      <c r="Q13">
-        <v>-29474000000</v>
-      </c>
-      <c r="R13">
-        <v>-1349000000</v>
-      </c>
-      <c r="S13">
-        <v>-1345000000</v>
-      </c>
-      <c r="T13">
-        <v>-1249000000</v>
-      </c>
-      <c r="U13">
-        <v>-1245000000</v>
-      </c>
-      <c r="V13">
-        <v>17765000000</v>
-      </c>
-      <c r="W13">
-        <v>17759000000</v>
-      </c>
-      <c r="X13">
-        <v>16500000000</v>
-      </c>
-      <c r="Y13">
-        <v>16480000000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2010</v>
       </c>
       <c r="B14">
+        <v>4562300</v>
+      </c>
+      <c r="C14">
+        <v>21400</v>
+      </c>
+      <c r="D14">
+        <v>77200</v>
+      </c>
+      <c r="E14">
+        <v>28400</v>
+      </c>
+      <c r="F14">
+        <v>48800</v>
+      </c>
+      <c r="G14">
+        <v>41800</v>
+      </c>
+      <c r="H14">
+        <v>69200</v>
+      </c>
+      <c r="I14">
+        <v>-27400</v>
+      </c>
+      <c r="J14">
+        <v>2262200</v>
+      </c>
+      <c r="K14">
+        <v>2292600</v>
+      </c>
+      <c r="L14">
+        <v>4554800</v>
+      </c>
+      <c r="M14">
         <v>200772000000</v>
       </c>
-      <c r="C14">
-        <v>203288000000</v>
-      </c>
-      <c r="D14">
-        <v>167392000000</v>
-      </c>
-      <c r="E14">
-        <v>167248000000</v>
-      </c>
-      <c r="F14">
+      <c r="N14">
         <v>171011000000</v>
       </c>
-      <c r="G14">
-        <v>172583000000</v>
-      </c>
-      <c r="H14">
-        <v>139440000000</v>
-      </c>
-      <c r="I14">
-        <v>139267000000</v>
-      </c>
-      <c r="J14">
+      <c r="O14">
         <v>184048000000</v>
       </c>
-      <c r="K14">
-        <v>186766000000</v>
-      </c>
-      <c r="L14">
-        <v>152193000000</v>
-      </c>
-      <c r="M14">
-        <v>152053000000</v>
-      </c>
-      <c r="N14">
-        <v>-30675000000</v>
-      </c>
-      <c r="O14">
-        <v>-30704000000</v>
-      </c>
-      <c r="P14">
-        <v>-27950000000</v>
-      </c>
-      <c r="Q14">
-        <v>-27981000000</v>
-      </c>
-      <c r="R14">
-        <v>-1211000000</v>
-      </c>
-      <c r="S14">
-        <v>-1204000000</v>
-      </c>
-      <c r="T14">
-        <v>-1110000000</v>
-      </c>
-      <c r="U14">
-        <v>-1103000000</v>
-      </c>
-      <c r="V14">
-        <v>17724000000</v>
-      </c>
-      <c r="W14">
-        <v>17727000000</v>
-      </c>
-      <c r="X14">
-        <v>16309000000</v>
-      </c>
-      <c r="Y14">
-        <v>16298000000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2011</v>
       </c>
       <c r="B15">
+        <v>4582400</v>
+      </c>
+      <c r="C15">
+        <v>20100</v>
+      </c>
+      <c r="D15">
+        <v>75100</v>
+      </c>
+      <c r="E15">
+        <v>27700</v>
+      </c>
+      <c r="F15">
+        <v>47400</v>
+      </c>
+      <c r="G15">
+        <v>53300</v>
+      </c>
+      <c r="H15">
+        <v>80600</v>
+      </c>
+      <c r="I15">
+        <v>-27300</v>
+      </c>
+      <c r="J15">
+        <v>2270500</v>
+      </c>
+      <c r="K15">
+        <v>2304400</v>
+      </c>
+      <c r="L15">
+        <v>4574900</v>
+      </c>
+      <c r="M15">
         <v>203343000000</v>
       </c>
-      <c r="C15">
-        <v>205729000000</v>
-      </c>
-      <c r="D15">
-        <v>171824000000</v>
-      </c>
-      <c r="E15">
-        <v>171740000000</v>
-      </c>
-      <c r="F15">
+      <c r="N15">
         <v>166763000000</v>
       </c>
-      <c r="G15">
-        <v>168861000000</v>
-      </c>
-      <c r="H15">
-        <v>138434000000</v>
-      </c>
-      <c r="I15">
-        <v>138340000000</v>
-      </c>
-      <c r="J15">
+      <c r="O15">
         <v>187495000000</v>
       </c>
-      <c r="K15">
-        <v>189949000000</v>
-      </c>
-      <c r="L15">
-        <v>156967000000</v>
-      </c>
-      <c r="M15">
-        <v>156857000000</v>
-      </c>
-      <c r="N15">
-        <v>-36829000000</v>
-      </c>
-      <c r="O15">
-        <v>-36867000000</v>
-      </c>
-      <c r="P15">
-        <v>-33389000000</v>
-      </c>
-      <c r="Q15">
-        <v>-33400000000</v>
-      </c>
-      <c r="R15">
-        <v>-1155000000</v>
-      </c>
-      <c r="S15">
-        <v>-1152000000</v>
-      </c>
-      <c r="T15">
-        <v>-1088000000</v>
-      </c>
-      <c r="U15">
-        <v>-1083000000</v>
-      </c>
-      <c r="V15">
-        <v>16902000000</v>
-      </c>
-      <c r="W15">
-        <v>16931000000</v>
-      </c>
-      <c r="X15">
-        <v>15945000000</v>
-      </c>
-      <c r="Y15">
-        <v>15965000000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2012</v>
       </c>
       <c r="B16">
+        <v>4601200</v>
+      </c>
+      <c r="C16">
+        <v>18800</v>
+      </c>
+      <c r="D16">
+        <v>73200</v>
+      </c>
+      <c r="E16">
+        <v>28700</v>
+      </c>
+      <c r="F16">
+        <v>44500</v>
+      </c>
+      <c r="G16">
+        <v>57300</v>
+      </c>
+      <c r="H16">
+        <v>83000</v>
+      </c>
+      <c r="I16">
+        <v>-25700</v>
+      </c>
+      <c r="J16">
+        <v>2275000</v>
+      </c>
+      <c r="K16">
+        <v>2318700</v>
+      </c>
+      <c r="L16">
+        <v>4593700</v>
+      </c>
+      <c r="M16">
         <v>203080000000</v>
       </c>
-      <c r="C16">
-        <v>205528000000</v>
-      </c>
-      <c r="D16">
-        <v>175219000000</v>
-      </c>
-      <c r="E16">
-        <v>174591000000</v>
-      </c>
-      <c r="F16">
+      <c r="N16">
         <v>166053000000</v>
       </c>
-      <c r="G16">
-        <v>168299000000</v>
-      </c>
-      <c r="H16">
-        <v>140248000000</v>
-      </c>
-      <c r="I16">
-        <v>139636000000</v>
-      </c>
-      <c r="J16">
+      <c r="O16">
         <v>187102000000</v>
       </c>
-      <c r="K16">
-        <v>189677000000</v>
-      </c>
-      <c r="L16">
-        <v>160005000000</v>
-      </c>
-      <c r="M16">
-        <v>159386000000</v>
-      </c>
-      <c r="N16">
-        <v>-37235000000</v>
-      </c>
-      <c r="O16">
-        <v>-37229000000</v>
-      </c>
-      <c r="P16">
-        <v>-34971000000</v>
-      </c>
-      <c r="Q16">
-        <v>-34955000000</v>
-      </c>
-      <c r="R16">
-        <v>-1176000000</v>
-      </c>
-      <c r="S16">
-        <v>-1171000000</v>
-      </c>
-      <c r="T16">
-        <v>-1127000000</v>
-      </c>
-      <c r="U16">
-        <v>-1120000000</v>
-      </c>
-      <c r="V16">
-        <v>17035000000</v>
-      </c>
-      <c r="W16">
-        <v>17022000000</v>
-      </c>
-      <c r="X16">
-        <v>16342000000</v>
-      </c>
-      <c r="Y16">
-        <v>16325000000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2013</v>
       </c>
       <c r="B17">
+        <v>4622200</v>
+      </c>
+      <c r="C17">
+        <v>21000</v>
+      </c>
+      <c r="D17">
+        <v>69400</v>
+      </c>
+      <c r="E17">
+        <v>29800</v>
+      </c>
+      <c r="F17">
+        <v>39600</v>
+      </c>
+      <c r="G17">
+        <v>62700</v>
+      </c>
+      <c r="H17">
+        <v>81300</v>
+      </c>
+      <c r="I17">
+        <v>-18600</v>
+      </c>
+      <c r="J17">
+        <v>2286100</v>
+      </c>
+      <c r="K17">
+        <v>2328500</v>
+      </c>
+      <c r="L17">
+        <v>4614600</v>
+      </c>
+      <c r="M17">
         <v>205466000000</v>
       </c>
-      <c r="C17">
-        <v>209177000000</v>
-      </c>
-      <c r="D17">
-        <v>179285000000</v>
-      </c>
-      <c r="E17">
-        <v>178813000000</v>
-      </c>
-      <c r="F17">
+      <c r="N17">
         <v>175230000000</v>
       </c>
-      <c r="G17">
-        <v>178005000000</v>
-      </c>
-      <c r="H17">
-        <v>150326000000</v>
-      </c>
-      <c r="I17">
-        <v>149869000000</v>
-      </c>
-      <c r="J17">
+      <c r="O17">
         <v>188780000000</v>
       </c>
-      <c r="K17">
-        <v>192713000000</v>
-      </c>
-      <c r="L17">
-        <v>163369000000</v>
-      </c>
-      <c r="M17">
-        <v>162943000000</v>
-      </c>
-      <c r="N17">
-        <v>-31173000000</v>
-      </c>
-      <c r="O17">
-        <v>-31173000000</v>
-      </c>
-      <c r="P17">
-        <v>-28958000000</v>
-      </c>
-      <c r="Q17">
-        <v>-28945000000</v>
-      </c>
-      <c r="R17">
-        <v>-1121000000</v>
-      </c>
-      <c r="S17">
-        <v>-1131000000</v>
-      </c>
-      <c r="T17">
-        <v>-1079000000</v>
-      </c>
-      <c r="U17">
-        <v>-1087000000</v>
-      </c>
-      <c r="V17">
-        <v>17630000000</v>
-      </c>
-      <c r="W17">
-        <v>17594000000</v>
-      </c>
-      <c r="X17">
-        <v>16995000000</v>
-      </c>
-      <c r="Y17">
-        <v>16958000000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2014</v>
       </c>
       <c r="B18">
+        <v>4652900</v>
+      </c>
+      <c r="C18">
+        <v>30700</v>
+      </c>
+      <c r="D18">
+        <v>68400</v>
+      </c>
+      <c r="E18">
+        <v>29200</v>
+      </c>
+      <c r="F18">
+        <v>39200</v>
+      </c>
+      <c r="G18">
+        <v>66500</v>
+      </c>
+      <c r="H18">
+        <v>75000</v>
+      </c>
+      <c r="I18">
+        <v>-8500</v>
+      </c>
+      <c r="J18">
+        <v>2299000</v>
+      </c>
+      <c r="K18">
+        <v>2346400</v>
+      </c>
+      <c r="L18">
+        <v>4645400</v>
+      </c>
+      <c r="M18">
         <v>223606000000</v>
       </c>
-      <c r="C18">
-        <v>226613000000</v>
-      </c>
-      <c r="D18">
-        <v>195471000000</v>
-      </c>
-      <c r="E18">
-        <v>195133000000</v>
-      </c>
-      <c r="F18">
+      <c r="N18">
         <v>191298000000</v>
       </c>
-      <c r="G18">
-        <v>193227000000</v>
-      </c>
-      <c r="H18">
-        <v>164357000000</v>
-      </c>
-      <c r="I18">
-        <v>163996000000</v>
-      </c>
-      <c r="J18">
+      <c r="O18">
         <v>205224000000</v>
       </c>
-      <c r="K18">
-        <v>208369000000</v>
-      </c>
-      <c r="L18">
-        <v>177924000000</v>
-      </c>
-      <c r="M18">
-        <v>177517000000</v>
-      </c>
-      <c r="N18">
-        <v>-33373000000</v>
-      </c>
-      <c r="O18">
-        <v>-33385000000</v>
-      </c>
-      <c r="P18">
-        <v>-31113000000</v>
-      </c>
-      <c r="Q18">
-        <v>-31137000000</v>
-      </c>
-      <c r="R18">
-        <v>-1017000000</v>
-      </c>
-      <c r="S18">
-        <v>-1021000000</v>
-      </c>
-      <c r="T18">
-        <v>-982000000</v>
-      </c>
-      <c r="U18">
-        <v>-985000000</v>
-      </c>
-      <c r="V18">
-        <v>19184000000</v>
-      </c>
-      <c r="W18">
-        <v>19265000000</v>
-      </c>
-      <c r="X18">
-        <v>18528000000</v>
-      </c>
-      <c r="Y18">
-        <v>18601000000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2015</v>
       </c>
       <c r="B19">
+        <v>4695300</v>
+      </c>
+      <c r="C19">
+        <v>42400</v>
+      </c>
+      <c r="D19">
+        <v>66400</v>
+      </c>
+      <c r="E19">
+        <v>29900</v>
+      </c>
+      <c r="F19">
+        <v>36500</v>
+      </c>
+      <c r="G19">
+        <v>75900</v>
+      </c>
+      <c r="H19">
+        <v>70000</v>
+      </c>
+      <c r="I19">
+        <v>5900</v>
+      </c>
+      <c r="J19">
+        <v>2317700</v>
+      </c>
+      <c r="K19">
+        <v>2370100</v>
+      </c>
+      <c r="L19">
+        <v>4687800</v>
+      </c>
+      <c r="M19">
         <v>278334000000</v>
       </c>
-      <c r="C19">
-        <v>276802000000</v>
-      </c>
-      <c r="D19">
-        <v>263507000000</v>
-      </c>
-      <c r="E19">
-        <v>263527000000</v>
-      </c>
-      <c r="F19">
+      <c r="N19">
         <v>215863000000</v>
       </c>
-      <c r="G19">
-        <v>214718000000</v>
-      </c>
-      <c r="H19">
-        <v>201727000000</v>
-      </c>
-      <c r="I19">
-        <v>201702000000</v>
-      </c>
-      <c r="J19">
+      <c r="O19">
         <v>258944000000</v>
       </c>
-      <c r="K19">
-        <v>257302000000</v>
-      </c>
-      <c r="L19">
-        <v>244748000000</v>
-      </c>
-      <c r="M19">
-        <v>244751000000</v>
-      </c>
-      <c r="N19">
-        <v>-62054000000</v>
-      </c>
-      <c r="O19">
-        <v>-62084000000</v>
-      </c>
-      <c r="P19">
-        <v>-61780000000</v>
-      </c>
-      <c r="Q19">
-        <v>-61826000000</v>
-      </c>
-      <c r="R19">
-        <v>-930000000</v>
-      </c>
-      <c r="S19">
-        <v>-931000000</v>
-      </c>
-      <c r="T19">
-        <v>-893000000</v>
-      </c>
-      <c r="U19">
-        <v>-895000000</v>
-      </c>
-      <c r="V19">
-        <v>20408000000</v>
-      </c>
-      <c r="W19">
-        <v>20431000000</v>
-      </c>
-      <c r="X19">
-        <v>19652000000</v>
-      </c>
-      <c r="Y19">
-        <v>19670000000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2016</v>
       </c>
       <c r="B20">
+        <v>4747000</v>
+      </c>
+      <c r="C20">
+        <v>51700</v>
+      </c>
+      <c r="D20">
+        <v>65400</v>
+      </c>
+      <c r="E20">
+        <v>29800</v>
+      </c>
+      <c r="F20">
+        <v>35600</v>
+      </c>
+      <c r="G20">
+        <v>82300</v>
+      </c>
+      <c r="H20">
+        <v>66200</v>
+      </c>
+      <c r="I20">
+        <v>16100</v>
+      </c>
+      <c r="J20">
+        <v>2346500</v>
+      </c>
+      <c r="K20">
+        <v>2393100</v>
+      </c>
+      <c r="L20">
+        <v>4739600</v>
+      </c>
+      <c r="M20">
         <v>283248000000</v>
       </c>
-      <c r="C20">
-        <v>283212000000</v>
-      </c>
-      <c r="D20">
-        <v>269725000000</v>
-      </c>
-      <c r="E20">
-        <v>268863000000</v>
-      </c>
-      <c r="F20">
+      <c r="N20">
         <v>231361000000</v>
       </c>
-      <c r="G20">
-        <v>230995000000</v>
-      </c>
-      <c r="H20">
-        <v>218882000000</v>
-      </c>
-      <c r="I20">
-        <v>217935000000</v>
-      </c>
-      <c r="J20">
+      <c r="O20">
         <v>262607000000</v>
       </c>
-      <c r="K20">
-        <v>262463000000</v>
-      </c>
-      <c r="L20">
-        <v>249776000000</v>
-      </c>
-      <c r="M20">
-        <v>248881000000</v>
-      </c>
-      <c r="N20">
-        <v>-52180000000</v>
-      </c>
-      <c r="O20">
-        <v>-52217000000</v>
-      </c>
-      <c r="P20">
-        <v>-50842000000</v>
-      </c>
-      <c r="Q20">
-        <v>-50928000000</v>
-      </c>
-      <c r="R20">
-        <v>-975000000</v>
-      </c>
-      <c r="S20">
-        <v>-976000000</v>
-      </c>
-      <c r="T20">
-        <v>-937000000</v>
-      </c>
-      <c r="U20">
-        <v>-938000000</v>
-      </c>
-      <c r="V20">
-        <v>21690000000</v>
-      </c>
-      <c r="W20">
-        <v>21728000000</v>
-      </c>
-      <c r="X20">
-        <v>20886000000</v>
-      </c>
-      <c r="Y20">
-        <v>20923000000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2017</v>
       </c>
       <c r="B21">
+        <v>4818300</v>
+      </c>
+      <c r="C21">
+        <v>71300</v>
+      </c>
+      <c r="D21">
+        <v>63400</v>
+      </c>
+      <c r="E21">
+        <v>31300</v>
+      </c>
+      <c r="F21">
+        <v>32100</v>
+      </c>
+      <c r="G21">
+        <v>95300</v>
+      </c>
+      <c r="H21">
+        <v>56100</v>
+      </c>
+      <c r="I21">
+        <v>39200</v>
+      </c>
+      <c r="J21">
+        <v>2380800</v>
+      </c>
+      <c r="K21">
+        <v>2430100</v>
+      </c>
+      <c r="L21">
+        <v>4810900</v>
+      </c>
+      <c r="M21">
         <v>309621000000</v>
       </c>
-      <c r="C21">
-        <v>311414000000</v>
-      </c>
-      <c r="D21">
-        <v>298529000000</v>
-      </c>
-      <c r="E21">
-        <v>297614000000</v>
-      </c>
-      <c r="F21">
+      <c r="N21">
         <v>246086000000</v>
       </c>
-      <c r="G21">
-        <v>247688000000</v>
-      </c>
-      <c r="H21">
-        <v>236490000000</v>
-      </c>
-      <c r="I21">
-        <v>235461000000</v>
-      </c>
-      <c r="J21">
+      <c r="O21">
         <v>288222000000</v>
       </c>
-      <c r="K21">
-        <v>289971000000</v>
-      </c>
-      <c r="L21">
-        <v>277760000000</v>
-      </c>
-      <c r="M21">
-        <v>276895000000</v>
-      </c>
-      <c r="N21">
-        <v>-63658000000</v>
-      </c>
-      <c r="O21">
-        <v>-63727000000</v>
-      </c>
-      <c r="P21">
-        <v>-62039000000</v>
-      </c>
-      <c r="Q21">
-        <v>-62153000000</v>
-      </c>
-      <c r="R21">
-        <v>-993000000</v>
-      </c>
-      <c r="S21">
-        <v>-994000000</v>
-      </c>
-      <c r="T21">
-        <v>-958000000</v>
-      </c>
-      <c r="U21">
-        <v>-960000000</v>
-      </c>
-      <c r="V21">
-        <v>22488000000</v>
-      </c>
-      <c r="W21">
-        <v>22439000000</v>
-      </c>
-      <c r="X21">
-        <v>21727000000</v>
-      </c>
-      <c r="Y21">
-        <v>21677000000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2018</v>
       </c>
       <c r="B22">
+        <v>4892300</v>
+      </c>
+      <c r="C22">
+        <v>74000</v>
+      </c>
+      <c r="D22">
+        <v>61600</v>
+      </c>
+      <c r="E22">
+        <v>32000</v>
+      </c>
+      <c r="F22">
+        <v>29600</v>
+      </c>
+      <c r="G22">
+        <v>96000</v>
+      </c>
+      <c r="H22">
+        <v>51600</v>
+      </c>
+      <c r="I22">
+        <v>44400</v>
+      </c>
+      <c r="J22">
+        <v>2419500</v>
+      </c>
+      <c r="K22">
+        <v>2465400</v>
+      </c>
+      <c r="L22">
+        <v>4884900</v>
+      </c>
+      <c r="M22">
         <v>335849000000</v>
       </c>
-      <c r="C22">
-        <v>338237000000</v>
-      </c>
-      <c r="D22">
-        <v>327441000000</v>
-      </c>
-      <c r="E22">
-        <v>327034000000</v>
-      </c>
-      <c r="F22">
+      <c r="N22">
         <v>260724000000</v>
       </c>
-      <c r="G22">
-        <v>262942000000</v>
-      </c>
-      <c r="H22">
-        <v>252978000000</v>
-      </c>
-      <c r="I22">
-        <v>252360000000</v>
-      </c>
-      <c r="J22">
+      <c r="O22">
         <v>313888000000</v>
       </c>
-      <c r="K22">
-        <v>316200000000</v>
-      </c>
-      <c r="L22">
-        <v>306014000000</v>
-      </c>
-      <c r="M22">
-        <v>305644000000</v>
-      </c>
-      <c r="N22">
-        <v>-75171000000</v>
-      </c>
-      <c r="O22">
-        <v>-75296000000</v>
-      </c>
-      <c r="P22">
-        <v>-74463000000</v>
-      </c>
-      <c r="Q22">
-        <v>-74674000000</v>
-      </c>
-      <c r="R22">
-        <v>-1054000000</v>
-      </c>
-      <c r="S22">
-        <v>-1055000000</v>
-      </c>
-      <c r="T22">
-        <v>-1022000000</v>
-      </c>
-      <c r="U22">
-        <v>-1024000000</v>
-      </c>
-      <c r="V22">
-        <v>23120000000</v>
-      </c>
-      <c r="W22">
-        <v>23094000000</v>
-      </c>
-      <c r="X22">
-        <v>22449000000</v>
-      </c>
-      <c r="Y22">
-        <v>22414000000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2019</v>
       </c>
       <c r="B23">
+        <v>4965900</v>
+      </c>
+      <c r="C23">
+        <v>73600</v>
+      </c>
+      <c r="D23">
+        <v>60500</v>
+      </c>
+      <c r="E23">
+        <v>30900</v>
+      </c>
+      <c r="F23">
+        <v>29600</v>
+      </c>
+      <c r="G23">
+        <v>97100</v>
+      </c>
+      <c r="H23">
+        <v>53100</v>
+      </c>
+      <c r="I23">
+        <v>44000</v>
+      </c>
+      <c r="J23">
+        <v>2456300</v>
+      </c>
+      <c r="K23">
+        <v>2502200</v>
+      </c>
+      <c r="L23">
+        <v>4958500</v>
+      </c>
+      <c r="M23">
         <v>353641000000</v>
       </c>
-      <c r="C23">
-        <v>357062000000</v>
-      </c>
-      <c r="D23">
-        <v>356357000000</v>
-      </c>
-      <c r="E23">
-        <v>355849000000</v>
-      </c>
-      <c r="F23">
+      <c r="N23">
         <v>273940000000</v>
       </c>
-      <c r="G23">
-        <v>277167000000</v>
-      </c>
-      <c r="H23">
-        <v>275583000000</v>
-      </c>
-      <c r="I23">
-        <v>274796000000</v>
-      </c>
-      <c r="J23">
+      <c r="O23">
         <v>330084000000</v>
       </c>
-      <c r="K23">
-        <v>333351000000</v>
-      </c>
-      <c r="L23">
-        <v>333161000000</v>
-      </c>
-      <c r="M23">
-        <v>332619000000</v>
-      </c>
-      <c r="N23">
-        <v>-79735000000</v>
-      </c>
-      <c r="O23">
-        <v>-79894000000</v>
-      </c>
-      <c r="P23">
-        <v>-80774000000</v>
-      </c>
-      <c r="Q23">
-        <v>-81052000000</v>
-      </c>
-      <c r="R23">
-        <v>-1072000000</v>
-      </c>
-      <c r="S23">
-        <v>-1071000000</v>
-      </c>
-      <c r="T23">
-        <v>-1049000000</v>
-      </c>
-      <c r="U23">
-        <v>-1049000000</v>
-      </c>
-      <c r="V23">
-        <v>24742000000</v>
-      </c>
-      <c r="W23">
-        <v>24782000000</v>
-      </c>
-      <c r="X23">
-        <v>24246000000</v>
-      </c>
-      <c r="Y23">
-        <v>24277000000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2020</v>
       </c>
       <c r="B24">
+        <v>5037300</v>
+      </c>
+      <c r="C24">
+        <v>71400</v>
+      </c>
+      <c r="D24">
+        <v>59100</v>
+      </c>
+      <c r="E24">
+        <v>32400</v>
+      </c>
+      <c r="F24">
+        <v>26700</v>
+      </c>
+      <c r="G24">
+        <v>95600</v>
+      </c>
+      <c r="H24">
+        <v>50900</v>
+      </c>
+      <c r="I24">
+        <v>44700</v>
+      </c>
+      <c r="J24">
+        <v>2491800</v>
+      </c>
+      <c r="K24">
+        <v>2538100</v>
+      </c>
+      <c r="L24">
+        <v>5029900</v>
+      </c>
+      <c r="M24">
         <v>377042000000</v>
       </c>
-      <c r="C24">
-        <v>377858000000</v>
-      </c>
-      <c r="D24">
-        <v>375250000000</v>
-      </c>
-      <c r="E24">
-        <v>375272000000</v>
-      </c>
-      <c r="F24">
+      <c r="N24">
         <v>283779000000</v>
       </c>
-      <c r="G24">
-        <v>284454000000</v>
-      </c>
-      <c r="H24">
-        <v>282917000000</v>
-      </c>
-      <c r="I24">
-        <v>282611000000</v>
-      </c>
-      <c r="J24">
+      <c r="O24">
         <v>356769000000</v>
       </c>
-      <c r="K24">
-        <v>357595000000</v>
-      </c>
-      <c r="L24">
-        <v>355478000000</v>
-      </c>
-      <c r="M24">
-        <v>355504000000</v>
-      </c>
-      <c r="N24">
-        <v>-93243000000</v>
-      </c>
-      <c r="O24">
-        <v>-93405000000</v>
-      </c>
-      <c r="P24">
-        <v>-92333000000</v>
-      </c>
-      <c r="Q24">
-        <v>-92663000000</v>
-      </c>
-      <c r="R24">
-        <v>-1397000000</v>
-      </c>
-      <c r="S24">
-        <v>-1400000000</v>
-      </c>
-      <c r="T24">
-        <v>-1361000000</v>
-      </c>
-      <c r="U24">
-        <v>-1366000000</v>
-      </c>
-      <c r="V24">
-        <v>21644000000</v>
-      </c>
-      <c r="W24">
-        <v>21662000000</v>
-      </c>
-      <c r="X24">
-        <v>21134000000</v>
-      </c>
-      <c r="Y24">
-        <v>21134000000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2021</v>
       </c>
       <c r="B25">
+        <v>5082100</v>
+      </c>
+      <c r="C25">
+        <v>44800</v>
+      </c>
+      <c r="D25">
+        <v>57300</v>
+      </c>
+      <c r="E25">
+        <v>34300</v>
+      </c>
+      <c r="F25">
+        <v>23000</v>
+      </c>
+      <c r="G25">
+        <v>74100</v>
+      </c>
+      <c r="H25">
+        <v>52300</v>
+      </c>
+      <c r="I25">
+        <v>21800</v>
+      </c>
+      <c r="J25">
+        <v>2514000</v>
+      </c>
+      <c r="K25">
+        <v>2560600</v>
+      </c>
+      <c r="L25">
+        <v>5074600</v>
+      </c>
+      <c r="M25">
         <v>434069000000</v>
       </c>
-      <c r="C25">
-        <v>433594000000</v>
-      </c>
-      <c r="D25">
-        <v>434070000000</v>
-      </c>
-      <c r="E25">
-        <v>433258000000</v>
-      </c>
-      <c r="F25">
+      <c r="N25">
         <v>323313000000</v>
       </c>
-      <c r="G25">
-        <v>322699000000</v>
-      </c>
-      <c r="H25">
-        <v>323314000000</v>
-      </c>
-      <c r="I25">
-        <v>322211000000</v>
-      </c>
-      <c r="J25">
+      <c r="O25">
         <v>409387000000</v>
       </c>
-      <c r="K25">
-        <v>408779000000</v>
-      </c>
-      <c r="L25">
-        <v>409386000000</v>
-      </c>
-      <c r="M25">
-        <v>408459000000</v>
-      </c>
-      <c r="N25">
-        <v>-110756000000</v>
-      </c>
-      <c r="O25">
-        <v>-110895000000</v>
-      </c>
-      <c r="P25">
-        <v>-110756000000</v>
-      </c>
-      <c r="Q25">
-        <v>-111046000000</v>
-      </c>
-      <c r="R25">
-        <v>-1662000000</v>
-      </c>
-      <c r="S25">
-        <v>-1659000000</v>
-      </c>
-      <c r="T25">
-        <v>-1661000000</v>
-      </c>
-      <c r="U25">
-        <v>-1659000000</v>
-      </c>
-      <c r="V25">
-        <v>26345000000</v>
-      </c>
-      <c r="W25">
-        <v>26475000000</v>
-      </c>
-      <c r="X25">
-        <v>26345000000</v>
-      </c>
-      <c r="Y25">
-        <v>26457000000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2022</v>
       </c>
       <c r="B26">
+        <v>5159900</v>
+      </c>
+      <c r="C26">
+        <v>77800</v>
+      </c>
+      <c r="D26">
+        <v>59700</v>
+      </c>
+      <c r="E26">
+        <v>33600</v>
+      </c>
+      <c r="F26">
+        <v>26100</v>
+      </c>
+      <c r="G26">
+        <v>107800</v>
+      </c>
+      <c r="H26">
+        <v>56100</v>
+      </c>
+      <c r="I26">
+        <v>51700</v>
+      </c>
+      <c r="J26">
+        <v>2562000</v>
+      </c>
+      <c r="K26">
+        <v>2622000</v>
+      </c>
+      <c r="L26">
+        <v>5184000</v>
+      </c>
+      <c r="M26">
         <v>475016000000</v>
       </c>
-      <c r="C26">
-        <v>474968000000</v>
-      </c>
-      <c r="D26">
-        <v>506282000000</v>
-      </c>
-      <c r="E26">
-        <v>506025000000</v>
-      </c>
-      <c r="F26">
+      <c r="N26">
         <v>335904000000</v>
       </c>
-      <c r="G26">
-        <v>335769000000</v>
-      </c>
-      <c r="H26">
-        <v>362876000000</v>
-      </c>
-      <c r="I26">
-        <v>362399000000</v>
-      </c>
-      <c r="J26">
+      <c r="O26">
         <v>450216000000</v>
-      </c>
-      <c r="K26">
-        <v>450233000000</v>
-      </c>
-      <c r="L26">
-        <v>479584000000</v>
-      </c>
-      <c r="M26">
-        <v>479389000000</v>
-      </c>
-      <c r="N26">
-        <v>-139112000000</v>
-      </c>
-      <c r="O26">
-        <v>-139201000000</v>
-      </c>
-      <c r="P26">
-        <v>-143406000000</v>
-      </c>
-      <c r="Q26">
-        <v>-143626000000</v>
-      </c>
-      <c r="R26">
-        <v>-1657000000</v>
-      </c>
-      <c r="S26">
-        <v>-1659000000</v>
-      </c>
-      <c r="T26">
-        <v>-1790000000</v>
-      </c>
-      <c r="U26">
-        <v>-1786000000</v>
-      </c>
-      <c r="V26">
-        <v>26459000000</v>
-      </c>
-      <c r="W26">
-        <v>26394000000</v>
-      </c>
-      <c r="X26">
-        <v>28487000000</v>
-      </c>
-      <c r="Y26">
-        <v>28425000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>